<commit_message>
Nuevas funciones en exportacion de pedidos.
</commit_message>
<xml_diff>
--- a/fieldex_cuenta_clientes.xlsx
+++ b/fieldex_cuenta_clientes.xlsx
@@ -29,7 +29,7 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
@@ -42,14 +42,8 @@
         <bgColor rgb="00FFFF00"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FFC7CE"/>
-        <bgColor rgb="00FFC7CE"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -57,22 +51,15 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -438,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -516,102 +503,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Barakat Vegetables And Fruits</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Fieldex</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>yuiyu</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>2024-01-04</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="n">
-        <v>13500</v>
-      </c>
-      <c r="G2" t="n">
-        <v>12500</v>
-      </c>
-      <c r="H2" t="n">
-        <v>20</v>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>2024-01-03</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>Abono</t>
-        </is>
-      </c>
-      <c r="K2" t="n">
-        <v>980</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="inlineStr">
-        <is>
-          <t>Barakat Vegetables And Fruits</t>
-        </is>
-      </c>
-      <c r="B3" s="2" t="inlineStr">
-        <is>
-          <t>Fieldex</t>
-        </is>
-      </c>
-      <c r="C3" s="2" t="inlineStr">
-        <is>
-          <t>-----------------</t>
-        </is>
-      </c>
-      <c r="D3" s="2" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="E3" s="2" t="inlineStr">
-        <is>
-          <t>Total Facturas</t>
-        </is>
-      </c>
-      <c r="F3" s="2" t="n">
-        <v>13500</v>
-      </c>
-      <c r="G3" s="2" t="inlineStr">
-        <is>
-          <t>Total Pagado Cliente</t>
-        </is>
-      </c>
-      <c r="H3" s="2" t="n">
-        <v>12500</v>
-      </c>
-      <c r="I3" s="2" t="inlineStr">
-        <is>
-          <t>Total Comisiones Banc</t>
-        </is>
-      </c>
-      <c r="J3" s="2" t="n">
-        <v>20</v>
-      </c>
-      <c r="K3" s="2" t="n">
-        <v>980</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>